<commit_message>
Fix mcu rotation in JLC prod file
</commit_message>
<xml_diff>
--- a/JLCPCB/JLCSMT_Sample_CPL1.xlsx
+++ b/JLCPCB/JLCSMT_Sample_CPL1.xlsx
@@ -436,11 +436,11 @@
   </sheetPr>
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K21" activeCellId="0" sqref="K21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E83" activeCellId="0" sqref="E83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.921875" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.18"/>
@@ -1857,7 +1857,7 @@
         <v>6</v>
       </c>
       <c r="E83" s="3" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>